<commit_message>
Modelagem de dados feita
</commit_message>
<xml_diff>
--- a/MODELAGEM DE DADOS/ModeloFisico.xlsx
+++ b/MODELAGEM DE DADOS/ModeloFisico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d431e4e78eb11568/Área de Trabalho/Senai/Projeto_Inicial-3T/MODELAGEM DE DADOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Desktop\Gustavo 3DT\Projeto_Inicial-3T\MODELAGEM DE DADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{2A772A66-A676-478F-8FD3-78C754AF6D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75D9C2E8-B3E1-4898-A2C4-0CFC2BFDA6AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B1323C-FD18-4503-854E-9EEC888F1404}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="7875" xr2:uid="{C9360F0B-1CC5-450A-A092-9FC21560DFF5}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="44">
   <si>
     <t>Usuarios</t>
   </si>
@@ -154,6 +145,18 @@
   </si>
   <si>
     <t>MackBook Air, 2TB, 4GB RAM I3 5° Geracao</t>
+  </si>
+  <si>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>IdEquipamento</t>
+  </si>
+  <si>
+    <t>HorarioEntrada</t>
+  </si>
+  <si>
+    <t>HorarioSaida</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +264,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -319,31 +340,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -659,17 +688,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9045D9-C5F3-4EB8-8563-1308669298C7}">
-  <dimension ref="B2:L14"/>
+  <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
@@ -680,34 +710,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="G2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -769,40 +799,40 @@
         <v>22</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="F11" s="13" t="s">
+      <c r="B11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -866,12 +896,49 @@
       </c>
       <c r="C14" s="1"/>
     </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="19">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="20">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="F10:L10"/>
+    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{1C795E16-F5C1-4270-9DFE-8EF83D357285}"/>

</xml_diff>